<commit_message>
feat: new model game_info
</commit_message>
<xml_diff>
--- a/Track.xlsx
+++ b/Track.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="154">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">https://api.nhle.com/stats/rest/en/team/summary?sort=shotsForPerGame&amp;cayenneExp=seasonId=20232024%20and%20gameTypeId=2</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_all_team_stats</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Standings</t>
   </si>
   <si>
@@ -75,6 +78,9 @@
     <t xml:space="preserve">https://api-web.nhle.com/v1/roster/TOR/20232024</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_roster_season</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Season</t>
   </si>
   <si>
@@ -105,36 +111,63 @@
     <t xml:space="preserve">https://api-web.nhle.com/v1/club-stats/TOR/20232024/2</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_all_club_stats</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Game Log</t>
   </si>
   <si>
     <t xml:space="preserve">https://api-web.nhle.com/v1/player/8478402/game-log/20232024/2</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_game_log</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Specific Player Info</t>
   </si>
   <si>
     <t xml:space="preserve">https://api-web.nhle.com/v1/player/8478402/landing</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_player_info</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Skater Stats</t>
   </si>
   <si>
     <t xml:space="preserve">https://api.nhle.com/stats/rest/en/skater/summary?limit=72&amp;start=17&amp;sort=points&amp;cayenneExp=seasonId=20232024</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_all_skaters_stats</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Goalie Stats</t>
   </si>
   <si>
     <t xml:space="preserve">https://api.nhle.com/stats/rest/en/goalie/summary?limit=72&amp;start=15&amp;sort=wins&amp;cayenneExp=seasonId=20232024</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_all_goalie_stats</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Game Information</t>
   </si>
   <si>
     <t xml:space="preserve">https://api.nhle.com/stats/rest/en/game</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_game_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Play by Play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://api-web.nhle.com/v1/gamecenter/2023020204/play-by-play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_play_by_play</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Game Log As of Now</t>
   </si>
   <si>
@@ -307,12 +340,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://api.nhle.com/stats/rest/en/glossary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Play by Play</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://api-web.nhle.com/v1/gamecenter/2023020204/play-by-play</t>
   </si>
   <si>
     <t xml:space="preserve">pk</t>
@@ -545,15 +572,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -680,21 +707,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="53.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="110.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="110.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="59.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="59.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="90.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="59.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="90.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="11.53"/>
   </cols>
@@ -761,7 +787,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>20232024</v>
@@ -773,218 +799,202 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>41</v>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -994,190 +1004,192 @@
         <v>51</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2"/>
+        <v>59</v>
+      </c>
       <c r="E27" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2"/>
+      <c r="E28" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="E29" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,7 +1200,7 @@
         <v>89</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,30 +1210,76 @@
       <c r="B41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>92</v>
+      <c r="C41" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>92</v>
+      <c r="C43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="E47" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1252,146 +1310,146 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>97</v>
+      <c r="A2" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>99</v>
+      <c r="A3" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>8478402</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>100</v>
+      <c r="A4" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>102</v>
+      <c r="A5" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>104</v>
+      <c r="A6" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>106</v>
+      <c r="A7" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>20152016</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>107</v>
+      <c r="A8" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>109</v>
+      <c r="A9" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>111</v>
+      <c r="A10" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>113</v>
+      <c r="A11" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>35443</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>114</v>
+      <c r="A12" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>116</v>
+      <c r="A13" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>118</v>
+      <c r="A14" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>185</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>119</v>
+      <c r="A15" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>120</v>
+      <c r="A16" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>121</v>
+      <c r="A17" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>193</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>122</v>
+      <c r="A18" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0"/>
+      <c r="B27" s="1"/>
       <c r="J27" s="5"/>
       <c r="AA27" s="5"/>
       <c r="AR27" s="5"/>
@@ -2381,178 +2439,178 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="16.18"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>97</v>
+      <c r="A5" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>847476520142015</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>99</v>
+      <c r="A6" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>8474765</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>106</v>
+      <c r="A7" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>20142015</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>124</v>
+      <c r="A8" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>102</v>
+      <c r="A9" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>111</v>
+      <c r="A10" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>127</v>
+      <c r="A11" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>128</v>
+      <c r="A12" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>129</v>
+      <c r="A13" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>130</v>
+      <c r="A14" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>131</v>
+      <c r="A15" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>132</v>
+      <c r="A16" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>725</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>133</v>
+      <c r="A17" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>135</v>
+      <c r="A18" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>136</v>
+      <c r="A19" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>138</v>
+      <c r="A20" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>139</v>
+      <c r="A21" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="B21" s="3" t="n">
         <v>84478</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>140</v>
+      <c r="A22" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B22" s="3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>141</v>
+      <c r="A23" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>142</v>
+      <c r="A24" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>143</v>
+      <c r="A25" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B25" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>144</v>
+      <c r="A26" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B26" s="3" t="n">
         <v>94</v>

</xml_diff>